<commit_message>
RESULTS FROM ANALYTICAL PROGRAM
</commit_message>
<xml_diff>
--- a/DataPlotter/FragilityFunction/2022/1.0.1/220211/ResultsSummary.xlsx
+++ b/DataPlotter/FragilityFunction/2022/1.0.1/220211/ResultsSummary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Concrete" sheetId="2" r:id="rId1"/>
@@ -558,7 +558,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -707,7 +706,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1243,7 +1241,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1378,7 +1375,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1930,6 +1926,7 @@
         <c:axId val="499536728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2072,8 +2069,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.2226386154855643"/>
-          <c:y val="0.46242490522018082"/>
+          <c:x val="0.21916639326334206"/>
+          <c:y val="5.9647127442403046E-2"/>
           <c:w val="0.28288194444444442"/>
           <c:h val="0.31415135608048994"/>
         </c:manualLayout>
@@ -2588,6 +2585,7 @@
         <c:axId val="499536728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4048,14 +4046,7 @@
                   <a:buFontTx/>
                   <a:buNone/>
                   <a:tabLst/>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
+                  <a:defRPr/>
                 </a:pPr>
                 <a:endParaRPr lang="en-US" sz="1100"/>
               </a:p>
@@ -10855,7 +10846,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>